<commit_message>
Invoice Classes has been changed
</commit_message>
<xml_diff>
--- a/Data/NetSuiteTestData_RemoveAgencyCommission.xlsx
+++ b/Data/NetSuiteTestData_RemoveAgencyCommission.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7515"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -97,46 +97,13 @@
     <t>TC_NST_2223</t>
   </si>
   <si>
-    <t>Split Invoice</t>
-  </si>
-  <si>
-    <t>TC_NST_6700</t>
-  </si>
-  <si>
-    <t>8215106224</t>
-  </si>
-  <si>
-    <t>TC_NST_6698</t>
-  </si>
-  <si>
     <t>iHeartmedia1!</t>
   </si>
   <si>
     <t>krishnagundavarapu@iheartmedia.com</t>
   </si>
   <si>
-    <t>TC_NST_6714</t>
-  </si>
-  <si>
-    <t>TC_NST_6699</t>
-  </si>
-  <si>
     <t>SB5 20.1 Upgrade - iHeartmedia  -  Administrator</t>
-  </si>
-  <si>
-    <t>8214958688</t>
-  </si>
-  <si>
-    <t>8215257050</t>
-  </si>
-  <si>
-    <t>TC_NST_6697</t>
-  </si>
-  <si>
-    <t>8215237089</t>
-  </si>
-  <si>
-    <t>8214957978</t>
   </si>
 </sst>
 </file>
@@ -528,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,13 +575,13 @@
         <v>3</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>11</v>
@@ -640,13 +607,13 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>11</v>
@@ -671,149 +638,29 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="G4" s="6"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="G5" s="6"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>39</v>
-      </c>
+      <c r="G6" s="6"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>36</v>
-      </c>
+      <c r="G7" s="6"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="G8" s="6"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -824,20 +671,10 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="D5" r:id="rId5"/>
-    <hyperlink ref="E2" r:id="rId6"/>
-    <hyperlink ref="E3" r:id="rId7"/>
-    <hyperlink ref="E4" r:id="rId8"/>
-    <hyperlink ref="E6" r:id="rId9"/>
-    <hyperlink ref="D6" r:id="rId10"/>
-    <hyperlink ref="E7" r:id="rId11"/>
-    <hyperlink ref="D7" r:id="rId12"/>
-    <hyperlink ref="D8" r:id="rId13"/>
-    <hyperlink ref="E8" r:id="rId14"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>